<commit_message>
DF Framework - Reports
</commit_message>
<xml_diff>
--- a/inputTestData/Accounts.xlsx
+++ b/inputTestData/Accounts.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\webautomation\inputTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96D13D7-6F6D-49AE-9478-177FEE47A607}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27CC28C-7F60-46EA-B1D8-F6DD67603DE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AccountHeirarchy (2)" sheetId="4" r:id="rId1"/>
-    <sheet name="AccountHeirarchy" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="AccountHeirarchy" sheetId="4" r:id="rId1"/>
+    <sheet name="AccountHeirarchy_RE" sheetId="1" r:id="rId2"/>
+    <sheet name="Template" sheetId="3" r:id="rId3"/>
     <sheet name="Users" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
   <si>
     <t>Parent</t>
   </si>
@@ -91,9 +91,6 @@
     <t>NORWAY</t>
   </si>
   <si>
-    <t>VTA1</t>
-  </si>
-  <si>
     <t>VTA2</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>VTA4</t>
   </si>
   <si>
-    <t>VTA5</t>
-  </si>
-  <si>
     <t>BANKID</t>
   </si>
   <si>
@@ -212,6 +206,81 @@
   </si>
   <si>
     <t>Virtual Cash Management</t>
+  </si>
+  <si>
+    <t>Report Type</t>
+  </si>
+  <si>
+    <t>Template Name</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Currencies</t>
+  </si>
+  <si>
+    <t>Amount Range</t>
+  </si>
+  <si>
+    <t>Transaction Type</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Account Owner Name</t>
+  </si>
+  <si>
+    <t>Shadow account name</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>Trans_</t>
+  </si>
+  <si>
+    <t>Select All</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Current month</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>-99999|99999999</t>
+  </si>
+  <si>
+    <t>Optional fields</t>
+  </si>
+  <si>
+    <t>Account name|Account Owner customer ID|Account Owner Name|Shadow account number|Shadow account name</t>
+  </si>
+  <si>
+    <t>Previous month</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Reporting Level</t>
+  </si>
+  <si>
+    <t>Include currency accounts</t>
+  </si>
+  <si>
+    <t>Bal_</t>
   </si>
 </sst>
 </file>
@@ -1064,324 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866C0B0-770D-4D07-95FE-682AE8FD2449}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-      <c r="U6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7">
-        <v>2</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>1.01</v>
-      </c>
-      <c r="P7">
-        <v>1.01</v>
-      </c>
-      <c r="U7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="U8" s="1"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1417,7 +1172,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1444,36 +1199,36 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>48</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>50</v>
-      </c>
-      <c r="P1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1488,13 +1243,13 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1518,7 +1273,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -1536,7 +1291,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1551,16 +1306,16 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -1574,20 +1329,276 @@
       <c r="I6" t="s">
         <v>16</v>
       </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1.01</v>
+      </c>
+      <c r="Q6">
+        <v>1.01</v>
+      </c>
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -1610,13 +1621,154 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B7A235-A154-4F92-B0C7-2AAE8A27A241}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="99.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1642,66 +1794,66 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F2" s="2">
         <v>1234567789</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reports changes to eliminate data dependancy
</commit_message>
<xml_diff>
--- a/inputTestData/Accounts.xlsx
+++ b/inputTestData/Accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\webautomation\inputTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27CC28C-7F60-46EA-B1D8-F6DD67603DE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EE48BA-3046-4ABC-A4EF-829222A0C41F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
   <si>
     <t>Parent</t>
   </si>
@@ -217,9 +217,6 @@
     <t>Access</t>
   </si>
   <si>
-    <t>Currencies</t>
-  </si>
-  <si>
     <t>Amount Range</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>Public</t>
   </si>
   <si>
-    <t>-99999|99999999</t>
-  </si>
-  <si>
     <t>Optional fields</t>
   </si>
   <si>
@@ -271,16 +265,13 @@
     <t>Previous month</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Reporting Level</t>
   </si>
   <si>
     <t>Include currency accounts</t>
   </si>
   <si>
-    <t>Bal_</t>
+    <t>-99999 - 99999999</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1127,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1621,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B7A235-A154-4F92-B0C7-2AAE8A27A241}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1633,7 +1624,7 @@
     <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
@@ -1655,115 +1646,110 @@
         <v>63</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>68</v>
-      </c>
-      <c r="M1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
       </c>
       <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
         <v>68</v>
-      </c>
-      <c r="M2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>70</v>
       </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
         <v>68</v>
-      </c>
-      <c r="M3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F5" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reports - Final version
</commit_message>
<xml_diff>
--- a/inputTestData/Accounts.xlsx
+++ b/inputTestData/Accounts.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\webautomation\inputTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EE48BA-3046-4ABC-A4EF-829222A0C41F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22CD37D-719B-4E72-8E43-CE8887F9843F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccountHeirarchy" sheetId="4" r:id="rId1"/>
     <sheet name="AccountHeirarchy_RE" sheetId="1" r:id="rId2"/>
-    <sheet name="Template" sheetId="3" r:id="rId3"/>
-    <sheet name="Users" sheetId="2" r:id="rId4"/>
+    <sheet name="Template_M" sheetId="5" r:id="rId3"/>
+    <sheet name="Template" sheetId="3" r:id="rId4"/>
+    <sheet name="Users" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
   <si>
     <t>Parent</t>
   </si>
@@ -226,12 +227,6 @@
     <t>Period</t>
   </si>
   <si>
-    <t>Account Owner Name</t>
-  </si>
-  <si>
-    <t>Shadow account name</t>
-  </si>
-  <si>
     <t>Transaction</t>
   </si>
   <si>
@@ -272,6 +267,18 @@
   </si>
   <si>
     <t>-99999 - 99999999</t>
+  </si>
+  <si>
+    <t>Select Schedule</t>
+  </si>
+  <si>
+    <t>Create Schedule to Run Later</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Every Week</t>
   </si>
 </sst>
 </file>
@@ -1611,11 +1618,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B7A235-A154-4F92-B0C7-2AAE8A27A241}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07C9663-317F-47E1-97EE-18F747F96F4A}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1631,11 +1638,9 @@
     <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="99.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -1652,7 +1657,7 @@
         <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1664,92 +1669,74 @@
         <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
         <v>73</v>
       </c>
-      <c r="I2" t="s">
-        <v>75</v>
-      </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="M2" t="s">
+      <c r="B3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1759,6 +1746,119 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B7A235-A154-4F92-B0C7-2AAE8A27A241}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="99.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6FC891-EC16-4EF7-983C-F26984448CA2}">
   <dimension ref="A1:J2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Delete/Block/Closed - Account scripts - Duplicate
</commit_message>
<xml_diff>
--- a/inputTestData/Accounts.xlsx
+++ b/inputTestData/Accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\webautomation\inputTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22CD37D-719B-4E72-8E43-CE8887F9843F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C75AA95-D721-4E82-9565-C9C5C7769675}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccountHeirarchy" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="88">
   <si>
     <t>Parent</t>
   </si>
@@ -92,9 +92,6 @@
     <t>NORWAY</t>
   </si>
   <si>
-    <t>VTA2</t>
-  </si>
-  <si>
     <t>VTA3</t>
   </si>
   <si>
@@ -279,6 +276,18 @@
   </si>
   <si>
     <t>Every Week</t>
+  </si>
+  <si>
+    <t>ShadowAcc</t>
+  </si>
+  <si>
+    <t>Root Acc</t>
+  </si>
+  <si>
+    <t>Agg One</t>
+  </si>
+  <si>
+    <t>Agg Two</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866C0B0-770D-4D07-95FE-682AE8FD2449}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1170,7 +1179,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1197,28 +1206,28 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>49</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
@@ -1229,7 +1238,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -1241,16 +1250,16 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -1268,13 +1277,13 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
@@ -1286,13 +1295,13 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -1304,16 +1313,16 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -1328,7 +1337,7 @@
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1355,16 +1364,16 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -1378,6 +1387,27 @@
       <c r="I7" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="V8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1426,7 +1456,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1453,36 +1483,36 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>49</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1497,13 +1527,13 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1527,7 +1557,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -1545,7 +1575,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1560,16 +1590,16 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -1587,16 +1617,16 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -1642,69 +1672,69 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
         <v>65</v>
       </c>
-      <c r="I1" t="s">
-        <v>66</v>
-      </c>
       <c r="J1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
@@ -1712,31 +1742,31 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1749,7 +1779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B7A235-A154-4F92-B0C7-2AAE8A27A241}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -1772,84 +1802,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
         <v>65</v>
       </c>
-      <c r="I1" t="s">
-        <v>66</v>
-      </c>
       <c r="J1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1880,66 +1910,66 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="2">
         <v>1234567789</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Customer verification methods
</commit_message>
<xml_diff>
--- a/inputTestData/Accounts.xlsx
+++ b/inputTestData/Accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\webautomation\inputTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09AAC52-6C3D-4B50-9458-02CC06CC3DE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4BAA96-ECE9-4CC4-8983-B2A856034721}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1652,7 +1652,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1779,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B7A235-A154-4F92-B0C7-2AAE8A27A241}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1893,7 +1893,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>